<commit_message>
22-02-24 site alarms check
</commit_message>
<xml_diff>
--- a/CMS/Site_Total_Alarms.xlsx
+++ b/CMS/Site_Total_Alarms.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,6 +490,31 @@
         <v>45</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>20240222</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>103</v>
+      </c>
+      <c r="C3" t="n">
+        <v>625</v>
+      </c>
+      <c r="D3" t="n">
+        <v>345</v>
+      </c>
+      <c r="E3" t="n">
+        <v>84</v>
+      </c>
+      <c r="F3" t="n">
+        <v>45</v>
+      </c>
+      <c r="G3" t="n">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added a script to run all and a graph creator
</commit_message>
<xml_diff>
--- a/CMS/Site_Total_Alarms.xlsx
+++ b/CMS/Site_Total_Alarms.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,6 +515,31 @@
         <v>92</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>20240223</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>174</v>
+      </c>
+      <c r="C4" t="n">
+        <v>674</v>
+      </c>
+      <c r="D4" t="n">
+        <v>345</v>
+      </c>
+      <c r="E4" t="n">
+        <v>86</v>
+      </c>
+      <c r="F4" t="n">
+        <v>45</v>
+      </c>
+      <c r="G4" t="n">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>